<commit_message>
Updating Myrtle beach strava
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\strava-inky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA3026-BDEF-49AA-8AC3-05C5A4952454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B81682-901B-41F2-A666-8B12A9E60BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="125">
   <si>
     <t>race</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>Cherry Blossom 10 Mile</t>
+  </si>
+  <si>
+    <t>myrtle_strava</t>
   </si>
 </sst>
 </file>
@@ -766,7 +769,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>